<commit_message>
Add json file,documentation for View.js and Position.js
</commit_message>
<xml_diff>
--- a/assets/addresses.xlsx
+++ b/assets/addresses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\TrustLook\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE755E1-6C1C-4665-B5CB-07ADDCAF67EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108197E3-8F2D-412E-B82A-5FF261B99B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -292,47 +292,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -653,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:A137"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,10 +1021,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A40:A57 A1:A29">
-    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:A102">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Account Worth add retry and token price comparison retry for account balance
</commit_message>
<xml_diff>
--- a/assets/addresses.xlsx
+++ b/assets/addresses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\TrustLook\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662386CF-508B-43B0-88ED-F7E271E68730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B94B860-9071-42DD-8DEF-94BA7F4E0516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,16 +17,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -316,17 +306,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -678,7 +658,7 @@
   <dimension ref="A1:A84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A72"/>
+      <selection activeCell="A3" sqref="A3:XFD72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,16 +1055,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A105:A115">
-    <cfRule type="duplicateValues" dxfId="5" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103:A104">
-    <cfRule type="duplicateValues" dxfId="4" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A102 A73:A74">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1463,7 +1443,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A72">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>